<commit_message>
Commit: changed export order
</commit_message>
<xml_diff>
--- a/BookingPortal/Files/export/AirBooking/du-lieu-dat-cho.xlsx
+++ b/BookingPortal/Files/export/AirBooking/du-lieu-dat-cho.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>DỮ LIỆU ĐẶT CHỖ 04/12/2020 - 04/12/2020</t>
   </si>
@@ -78,18 +78,6 @@
   </si>
   <si>
     <t>CWUGGX</t>
-  </si>
-  <si>
-    <t>FL1</t>
-  </si>
-  <si>
-    <t>dl01 tickting 01</t>
-  </si>
-  <si>
-    <t>KOVSJI</t>
-  </si>
-  <si>
-    <t>KOZZVT</t>
   </si>
 </sst>
 </file>
@@ -202,7 +190,7 @@
   <sheetPr>
     <tabColor rgb="FF000000"/>
   </sheetPr>
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -338,13 +326,13 @@
         <v>21</v>
       </c>
       <c r="I3" s="3">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J3" s="7">
         <v>2636000</v>
       </c>
       <c r="K3" s="7">
-        <v>0</v>
+        <v>200000</v>
       </c>
       <c r="L3" s="8">
         <v>0</v>
@@ -353,95 +341,7 @@
         <v>100000</v>
       </c>
       <c r="N3" s="8">
-        <v>2736000</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="3">
-        <v>2</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="I4" s="3">
-        <v>10</v>
-      </c>
-      <c r="J4" s="7">
-        <v>2683000</v>
-      </c>
-      <c r="K4" s="7">
-        <v>0</v>
-      </c>
-      <c r="L4" s="8">
-        <v>101000</v>
-      </c>
-      <c r="M4" s="8">
-        <v>150000</v>
-      </c>
-      <c r="N4" s="8">
-        <v>2934000</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="3">
-        <v>3</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="I5" s="3">
-        <v>11</v>
-      </c>
-      <c r="J5" s="7">
-        <v>2636000</v>
-      </c>
-      <c r="K5" s="7">
-        <v>0</v>
-      </c>
-      <c r="L5" s="8">
-        <v>101000</v>
-      </c>
-      <c r="M5" s="8">
-        <v>150000</v>
-      </c>
-      <c r="N5" s="8">
-        <v>2887000</v>
+        <v>2936000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>